<commit_message>
I have add SRG for topbreak also
</commit_message>
<xml_diff>
--- a/Forsta_meta.xlsx
+++ b/Forsta_meta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Internal\Tabulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D82D86-02A8-4F28-A392-325975691F66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6454B1D-B9C1-4085-8C3B-99A966D7DA8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="214">
   <si>
     <t>Var_Name</t>
   </si>
@@ -316,21 +316,6 @@
     <t>E11: Single select</t>
   </si>
   <si>
-    <t>E10r1: Family - Multi select</t>
-  </si>
-  <si>
-    <t>E10r2: Education - Multi select</t>
-  </si>
-  <si>
-    <t>E10r3: Health and fitness - Multi select</t>
-  </si>
-  <si>
-    <t>E10r4: Financial stability - Multi select</t>
-  </si>
-  <si>
-    <t>E10r5: Social life - Multi select</t>
-  </si>
-  <si>
     <t>E8: Open end</t>
   </si>
   <si>
@@ -463,264 +448,24 @@
     <t xml:space="preserve"> Single select</t>
   </si>
   <si>
-    <t xml:space="preserve"> Family - Multi select</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Education - Multi select</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Health and fitness - Multi select</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Financial stability - Multi select</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Social life - Multi select</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Open end</t>
   </si>
   <si>
     <t xml:space="preserve"> Numeric</t>
   </si>
   <si>
-    <t xml:space="preserve"> Exercise - Single select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Reading - Single select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cooking - Single select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Watching TV - Single select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Amazon - Electronics - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ASOS - Electronics - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Barnes &amp; Noble - Electronics - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Flipkart - Electronics - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Myntra - Electronics - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> JioMart - Electronics - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pepperfry - Electronics - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Amazon - Clothing - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ASOS - Clothing - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Barnes &amp; Noble - Clothing - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Flipkart - Clothing - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Myntra - Clothing - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> JioMart - Clothing - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pepperfry - Clothing - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Amazon - Groceries - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ASOS - Groceries - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Barnes &amp; Noble - Groceries - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Flipkart - Groceries - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Myntra - Groceries - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> JioMart - Groceries - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pepperfry - Groceries - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Amazon - Books - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ASOS - Books - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Barnes &amp; Noble - Books - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Flipkart - Books - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Myntra - Books - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> JioMart - Books - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pepperfry - Books - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Amazon - Home decor - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ASOS - Home decor - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Barnes &amp; Noble - Home decor - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Flipkart - Home decor - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Myntra - Home decor - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> JioMart - Home decor - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pepperfry - Home decor - Multi select grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Customer Support - Open end grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Product Quality - Open end grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Delivery Speed - Open end grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Website Usability - Open end grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Petrol - Numeric grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Electricity Bill - Numeric grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Water Bill - Numeric grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Vegetables - Numeric grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Groceries - Numeric grid</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 5 points scale rating</t>
   </si>
   <si>
-    <t xml:space="preserve"> Row 1 - 5 points scale rating grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Row 2 - 5 points scale rating grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Row 3 - 5 points scale rating grid</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 7 points scale rating</t>
   </si>
   <si>
-    <t xml:space="preserve"> Row 1 - 7 points scale rating grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Row 2 - 7 points scale rating grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Row 3 - 7 points scale rating grid</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 10 points scale rating</t>
   </si>
   <si>
-    <t xml:space="preserve"> Row 1 - 10 points scale rating grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Row 2 - 10 points scale rating grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Row 3 - 10 points scale rating grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LINE - Top 3 Rank</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> WhatsApp - Top 3 Rank</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Any other messenger (WeChat, messenger etc.) - Top 3 Rank</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Facebook - Top 3 Rank</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Other social media - Instagram - Top 3 Rank</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> YouTube - Top 3 Rank</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Google and other search engines - Top 3 Rank</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Columns 1 - Row 1 - Multi column dropdown</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Columns 2 - Row 1 - Multi column dropdown</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Columns 1 - Row 2 - Multi column dropdown</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Columns 2 - Row 2 - Multi column dropdown</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Columns 1 - Row 3 - Multi column dropdown</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Columns 2 - Row 3 - Multi column dropdown</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Columns 1 - Row 4 - Multi column dropdown</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Columns 2 - Row 4 - Multi column dropdown</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Net Promoter Score (NPS)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Row 1 - Net Promoter Score (NPS) grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Row 2 - Net Promoter Score (NPS) grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Row 3 - Net Promoter Score (NPS) grid</t>
-  </si>
-  <si>
     <t>OE</t>
   </si>
   <si>
@@ -806,6 +551,120 @@
   </si>
   <si>
     <t>E30</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Family</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Education</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Health and fitness</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Financial stability</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Social life</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Exercise</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Reading</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cooking</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Watching TV</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Customer Support</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Product Quality</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Delivery Speed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Website Usability</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Amazon </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ASOS </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Barnes &amp; Noble </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Flipkart </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Myntra </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> JioMart </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pepperfry </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Petrol </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Electricity Bill </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Water Bill </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vegetables </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Groceries </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Row 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Row 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Row 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LINE </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> WhatsApp </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Any other messenger (WeChat, messenger etc.) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Facebook </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Other social media </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> YouTube </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Google and other search engines </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Columns 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Columns 2 </t>
+  </si>
+  <si>
+    <t>E10:Multi select</t>
   </si>
 </sst>
 </file>
@@ -1175,14 +1034,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="G86" sqref="G86"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
@@ -1218,13 +1075,13 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C2" t="s">
         <v>95</v>
       </c>
       <c r="D2" t="s">
-        <v>232</v>
+        <v>147</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -1235,13 +1092,13 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C3" t="s">
         <v>96</v>
       </c>
       <c r="D3" t="s">
-        <v>233</v>
+        <v>148</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -1252,16 +1109,16 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>176</v>
       </c>
       <c r="C4" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="D4" t="s">
-        <v>234</v>
+        <v>149</v>
       </c>
       <c r="E4" t="s">
-        <v>243</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1269,16 +1126,16 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>147</v>
+        <v>177</v>
       </c>
       <c r="C5" t="s">
-        <v>98</v>
+        <v>213</v>
       </c>
       <c r="D5" t="s">
-        <v>234</v>
+        <v>149</v>
       </c>
       <c r="E5" t="s">
-        <v>243</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1286,16 +1143,16 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>148</v>
+        <v>178</v>
       </c>
       <c r="C6" t="s">
-        <v>99</v>
+        <v>213</v>
       </c>
       <c r="D6" t="s">
-        <v>234</v>
+        <v>149</v>
       </c>
       <c r="E6" t="s">
-        <v>243</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1303,16 +1160,16 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C7" t="s">
+        <v>213</v>
+      </c>
+      <c r="D7" t="s">
         <v>149</v>
       </c>
-      <c r="C7" t="s">
-        <v>100</v>
-      </c>
-      <c r="D7" t="s">
-        <v>234</v>
-      </c>
       <c r="E7" t="s">
-        <v>243</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1320,16 +1177,16 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="C8" t="s">
-        <v>101</v>
+        <v>213</v>
       </c>
       <c r="D8" t="s">
-        <v>234</v>
+        <v>149</v>
       </c>
       <c r="E8" t="s">
-        <v>243</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1337,13 +1194,13 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="C9" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D9" t="s">
-        <v>232</v>
+        <v>147</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
@@ -1354,13 +1211,13 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C10" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D10" t="s">
-        <v>235</v>
+        <v>150</v>
       </c>
       <c r="E10" t="s">
         <v>15</v>
@@ -1371,19 +1228,19 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>153</v>
+        <v>181</v>
       </c>
       <c r="C11" t="s">
-        <v>244</v>
+        <v>159</v>
       </c>
       <c r="D11" t="s">
-        <v>236</v>
+        <v>151</v>
       </c>
       <c r="E11" t="s">
-        <v>245</v>
+        <v>160</v>
       </c>
       <c r="G11" t="s">
-        <v>246</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1391,19 +1248,19 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="C12" t="s">
-        <v>244</v>
+        <v>159</v>
       </c>
       <c r="D12" t="s">
-        <v>236</v>
+        <v>151</v>
       </c>
       <c r="E12" t="s">
-        <v>245</v>
+        <v>160</v>
       </c>
       <c r="G12" t="s">
-        <v>246</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1411,19 +1268,19 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>155</v>
+        <v>183</v>
       </c>
       <c r="C13" t="s">
-        <v>244</v>
+        <v>159</v>
       </c>
       <c r="D13" t="s">
-        <v>236</v>
+        <v>151</v>
       </c>
       <c r="E13" t="s">
-        <v>245</v>
+        <v>160</v>
       </c>
       <c r="G13" t="s">
-        <v>246</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1431,19 +1288,19 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>156</v>
+        <v>184</v>
       </c>
       <c r="C14" t="s">
-        <v>244</v>
+        <v>159</v>
       </c>
       <c r="D14" t="s">
-        <v>236</v>
+        <v>151</v>
       </c>
       <c r="E14" t="s">
-        <v>245</v>
+        <v>160</v>
       </c>
       <c r="G14" t="s">
-        <v>246</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1451,16 +1308,16 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>157</v>
+        <v>189</v>
       </c>
       <c r="C15" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="D15" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E15" t="s">
-        <v>248</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1468,16 +1325,16 @@
         <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>158</v>
+        <v>190</v>
       </c>
       <c r="C16" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="D16" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E16" t="s">
-        <v>248</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1485,16 +1342,16 @@
         <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>159</v>
+        <v>191</v>
       </c>
       <c r="C17" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="D17" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E17" t="s">
-        <v>248</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1502,16 +1359,16 @@
         <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>160</v>
+        <v>192</v>
       </c>
       <c r="C18" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="D18" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E18" t="s">
-        <v>248</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1519,16 +1376,16 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>161</v>
+        <v>193</v>
       </c>
       <c r="C19" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="D19" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E19" t="s">
-        <v>248</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1536,16 +1393,16 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>162</v>
+        <v>194</v>
       </c>
       <c r="C20" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="D20" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E20" t="s">
-        <v>248</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1553,16 +1410,16 @@
         <v>26</v>
       </c>
       <c r="B21" t="s">
+        <v>195</v>
+      </c>
+      <c r="C21" t="s">
+        <v>162</v>
+      </c>
+      <c r="D21" t="s">
+        <v>152</v>
+      </c>
+      <c r="E21" t="s">
         <v>163</v>
-      </c>
-      <c r="C21" t="s">
-        <v>247</v>
-      </c>
-      <c r="D21" t="s">
-        <v>237</v>
-      </c>
-      <c r="E21" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1570,16 +1427,16 @@
         <v>27</v>
       </c>
       <c r="B22" t="s">
+        <v>189</v>
+      </c>
+      <c r="C22" t="s">
+        <v>162</v>
+      </c>
+      <c r="D22" t="s">
+        <v>152</v>
+      </c>
+      <c r="E22" t="s">
         <v>164</v>
-      </c>
-      <c r="C22" t="s">
-        <v>247</v>
-      </c>
-      <c r="D22" t="s">
-        <v>237</v>
-      </c>
-      <c r="E22" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1587,16 +1444,16 @@
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>165</v>
+        <v>190</v>
       </c>
       <c r="C23" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="D23" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E23" t="s">
-        <v>249</v>
+        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1604,16 +1461,16 @@
         <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>166</v>
+        <v>191</v>
       </c>
       <c r="C24" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="D24" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E24" t="s">
-        <v>249</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1621,16 +1478,16 @@
         <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>167</v>
+        <v>192</v>
       </c>
       <c r="C25" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="D25" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E25" t="s">
-        <v>249</v>
+        <v>164</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1638,16 +1495,16 @@
         <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>168</v>
+        <v>193</v>
       </c>
       <c r="C26" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="D26" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E26" t="s">
-        <v>249</v>
+        <v>164</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1655,16 +1512,16 @@
         <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>169</v>
+        <v>194</v>
       </c>
       <c r="C27" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="D27" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E27" t="s">
-        <v>249</v>
+        <v>164</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1672,16 +1529,16 @@
         <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>170</v>
+        <v>195</v>
       </c>
       <c r="C28" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="D28" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E28" t="s">
-        <v>249</v>
+        <v>164</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1689,16 +1546,16 @@
         <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>171</v>
+        <v>189</v>
       </c>
       <c r="C29" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="D29" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E29" t="s">
-        <v>250</v>
+        <v>165</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1706,16 +1563,16 @@
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>172</v>
+        <v>190</v>
       </c>
       <c r="C30" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="D30" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E30" t="s">
-        <v>250</v>
+        <v>165</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1723,16 +1580,16 @@
         <v>36</v>
       </c>
       <c r="B31" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
       <c r="C31" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="D31" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E31" t="s">
-        <v>250</v>
+        <v>165</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1740,16 +1597,16 @@
         <v>37</v>
       </c>
       <c r="B32" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="C32" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="D32" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E32" t="s">
-        <v>250</v>
+        <v>165</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1757,16 +1614,16 @@
         <v>38</v>
       </c>
       <c r="B33" t="s">
-        <v>175</v>
+        <v>193</v>
       </c>
       <c r="C33" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="D33" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E33" t="s">
-        <v>250</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1774,16 +1631,16 @@
         <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>176</v>
+        <v>194</v>
       </c>
       <c r="C34" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="D34" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E34" t="s">
-        <v>250</v>
+        <v>165</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1791,16 +1648,16 @@
         <v>40</v>
       </c>
       <c r="B35" t="s">
-        <v>177</v>
+        <v>195</v>
       </c>
       <c r="C35" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="D35" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E35" t="s">
-        <v>250</v>
+        <v>165</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1808,16 +1665,16 @@
         <v>41</v>
       </c>
       <c r="B36" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="C36" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="D36" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E36" t="s">
-        <v>251</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1825,16 +1682,16 @@
         <v>42</v>
       </c>
       <c r="B37" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="C37" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="D37" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E37" t="s">
-        <v>251</v>
+        <v>166</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1842,16 +1699,16 @@
         <v>43</v>
       </c>
       <c r="B38" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="C38" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="D38" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E38" t="s">
-        <v>251</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1859,16 +1716,16 @@
         <v>44</v>
       </c>
       <c r="B39" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
       <c r="C39" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="D39" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E39" t="s">
-        <v>251</v>
+        <v>166</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1876,16 +1733,16 @@
         <v>45</v>
       </c>
       <c r="B40" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
       <c r="C40" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="D40" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E40" t="s">
-        <v>251</v>
+        <v>166</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1893,16 +1750,16 @@
         <v>46</v>
       </c>
       <c r="B41" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="C41" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="D41" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E41" t="s">
-        <v>251</v>
+        <v>166</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1910,16 +1767,16 @@
         <v>47</v>
       </c>
       <c r="B42" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="C42" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="D42" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E42" t="s">
-        <v>251</v>
+        <v>166</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1927,16 +1784,16 @@
         <v>48</v>
       </c>
       <c r="B43" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="C43" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="D43" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E43" t="s">
-        <v>252</v>
+        <v>167</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1944,16 +1801,16 @@
         <v>49</v>
       </c>
       <c r="B44" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="C44" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="D44" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E44" t="s">
-        <v>252</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1961,16 +1818,16 @@
         <v>50</v>
       </c>
       <c r="B45" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C45" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="D45" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E45" t="s">
-        <v>252</v>
+        <v>167</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1978,16 +1835,16 @@
         <v>51</v>
       </c>
       <c r="B46" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="C46" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="D46" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E46" t="s">
-        <v>252</v>
+        <v>167</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1995,16 +1852,16 @@
         <v>52</v>
       </c>
       <c r="B47" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="C47" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="D47" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E47" t="s">
-        <v>252</v>
+        <v>167</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -2012,16 +1869,16 @@
         <v>53</v>
       </c>
       <c r="B48" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="C48" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="D48" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E48" t="s">
-        <v>252</v>
+        <v>167</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -2029,16 +1886,16 @@
         <v>54</v>
       </c>
       <c r="B49" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="C49" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="D49" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E49" t="s">
-        <v>252</v>
+        <v>167</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -2046,16 +1903,16 @@
         <v>55</v>
       </c>
       <c r="B50" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="C50" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D50" t="s">
-        <v>238</v>
+        <v>153</v>
       </c>
       <c r="E50" t="s">
-        <v>254</v>
+        <v>169</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -2063,16 +1920,16 @@
         <v>56</v>
       </c>
       <c r="B51" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="C51" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D51" t="s">
-        <v>238</v>
+        <v>153</v>
       </c>
       <c r="E51" t="s">
-        <v>254</v>
+        <v>169</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -2080,16 +1937,16 @@
         <v>57</v>
       </c>
       <c r="B52" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="C52" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D52" t="s">
-        <v>238</v>
+        <v>153</v>
       </c>
       <c r="E52" t="s">
-        <v>254</v>
+        <v>169</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -2097,16 +1954,16 @@
         <v>58</v>
       </c>
       <c r="B53" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="C53" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D53" t="s">
-        <v>238</v>
+        <v>153</v>
       </c>
       <c r="E53" t="s">
-        <v>254</v>
+        <v>169</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -2117,13 +1974,13 @@
         <v>196</v>
       </c>
       <c r="C54" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D54" t="s">
-        <v>239</v>
+        <v>154</v>
       </c>
       <c r="E54" t="s">
-        <v>255</v>
+        <v>170</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -2134,13 +1991,13 @@
         <v>197</v>
       </c>
       <c r="C55" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D55" t="s">
-        <v>239</v>
+        <v>154</v>
       </c>
       <c r="E55" t="s">
-        <v>255</v>
+        <v>170</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -2151,13 +2008,13 @@
         <v>198</v>
       </c>
       <c r="C56" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D56" t="s">
-        <v>239</v>
+        <v>154</v>
       </c>
       <c r="E56" t="s">
-        <v>255</v>
+        <v>170</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -2168,13 +2025,13 @@
         <v>199</v>
       </c>
       <c r="C57" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D57" t="s">
-        <v>239</v>
+        <v>154</v>
       </c>
       <c r="E57" t="s">
-        <v>255</v>
+        <v>170</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -2185,13 +2042,13 @@
         <v>200</v>
       </c>
       <c r="C58" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D58" t="s">
-        <v>239</v>
+        <v>154</v>
       </c>
       <c r="E58" t="s">
-        <v>255</v>
+        <v>170</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -2199,19 +2056,19 @@
         <v>64</v>
       </c>
       <c r="B59" t="s">
-        <v>201</v>
+        <v>143</v>
       </c>
       <c r="C59" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D59" t="s">
-        <v>233</v>
+        <v>148</v>
       </c>
       <c r="E59" t="s">
         <v>64</v>
       </c>
       <c r="G59" t="s">
-        <v>240</v>
+        <v>155</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -2219,19 +2076,19 @@
         <v>65</v>
       </c>
       <c r="B60" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C60" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D60" t="s">
-        <v>236</v>
+        <v>151</v>
       </c>
       <c r="E60" t="s">
-        <v>256</v>
+        <v>171</v>
       </c>
       <c r="G60" t="s">
-        <v>240</v>
+        <v>155</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -2239,19 +2096,19 @@
         <v>66</v>
       </c>
       <c r="B61" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C61" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D61" t="s">
-        <v>236</v>
+        <v>151</v>
       </c>
       <c r="E61" t="s">
-        <v>256</v>
+        <v>171</v>
       </c>
       <c r="G61" t="s">
-        <v>240</v>
+        <v>155</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -2259,19 +2116,19 @@
         <v>67</v>
       </c>
       <c r="B62" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C62" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D62" t="s">
-        <v>236</v>
+        <v>151</v>
       </c>
       <c r="E62" t="s">
-        <v>256</v>
+        <v>171</v>
       </c>
       <c r="G62" t="s">
-        <v>240</v>
+        <v>155</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -2279,19 +2136,19 @@
         <v>68</v>
       </c>
       <c r="B63" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="C63" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D63" t="s">
-        <v>233</v>
+        <v>148</v>
       </c>
       <c r="E63" t="s">
         <v>68</v>
       </c>
       <c r="G63" t="s">
-        <v>240</v>
+        <v>155</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -2299,19 +2156,19 @@
         <v>69</v>
       </c>
       <c r="B64" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C64" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D64" t="s">
-        <v>236</v>
+        <v>151</v>
       </c>
       <c r="E64" t="s">
-        <v>257</v>
+        <v>172</v>
       </c>
       <c r="G64" t="s">
-        <v>240</v>
+        <v>155</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -2319,19 +2176,19 @@
         <v>70</v>
       </c>
       <c r="B65" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C65" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D65" t="s">
-        <v>236</v>
+        <v>151</v>
       </c>
       <c r="E65" t="s">
-        <v>257</v>
+        <v>172</v>
       </c>
       <c r="G65" t="s">
-        <v>240</v>
+        <v>155</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -2339,19 +2196,19 @@
         <v>71</v>
       </c>
       <c r="B66" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C66" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D66" t="s">
-        <v>236</v>
+        <v>151</v>
       </c>
       <c r="E66" t="s">
-        <v>257</v>
+        <v>172</v>
       </c>
       <c r="G66" t="s">
-        <v>240</v>
+        <v>155</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -2359,19 +2216,19 @@
         <v>72</v>
       </c>
       <c r="B67" t="s">
-        <v>209</v>
+        <v>145</v>
       </c>
       <c r="C67" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D67" t="s">
-        <v>233</v>
+        <v>148</v>
       </c>
       <c r="E67" t="s">
         <v>72</v>
       </c>
       <c r="G67" t="s">
-        <v>240</v>
+        <v>155</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -2379,19 +2236,19 @@
         <v>73</v>
       </c>
       <c r="B68" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="C68" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D68" t="s">
-        <v>236</v>
+        <v>151</v>
       </c>
       <c r="E68" t="s">
-        <v>258</v>
+        <v>173</v>
       </c>
       <c r="G68" t="s">
-        <v>240</v>
+        <v>155</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -2399,19 +2256,19 @@
         <v>74</v>
       </c>
       <c r="B69" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C69" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D69" t="s">
-        <v>236</v>
+        <v>151</v>
       </c>
       <c r="E69" t="s">
-        <v>258</v>
+        <v>173</v>
       </c>
       <c r="G69" t="s">
-        <v>240</v>
+        <v>155</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -2419,19 +2276,19 @@
         <v>75</v>
       </c>
       <c r="B70" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C70" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D70" t="s">
-        <v>236</v>
+        <v>151</v>
       </c>
       <c r="E70" t="s">
-        <v>258</v>
+        <v>173</v>
       </c>
       <c r="G70" t="s">
-        <v>240</v>
+        <v>155</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -2439,19 +2296,19 @@
         <v>76</v>
       </c>
       <c r="B71" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C71" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D71" t="s">
-        <v>236</v>
+        <v>151</v>
       </c>
       <c r="E71" t="s">
-        <v>259</v>
+        <v>174</v>
       </c>
       <c r="G71" t="s">
-        <v>241</v>
+        <v>156</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -2459,19 +2316,19 @@
         <v>77</v>
       </c>
       <c r="B72" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C72" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D72" t="s">
-        <v>236</v>
+        <v>151</v>
       </c>
       <c r="E72" t="s">
-        <v>259</v>
+        <v>174</v>
       </c>
       <c r="G72" t="s">
-        <v>241</v>
+        <v>156</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -2479,19 +2336,19 @@
         <v>78</v>
       </c>
       <c r="B73" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C73" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D73" t="s">
-        <v>236</v>
+        <v>151</v>
       </c>
       <c r="E73" t="s">
-        <v>259</v>
+        <v>174</v>
       </c>
       <c r="G73" t="s">
-        <v>241</v>
+        <v>156</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -2499,19 +2356,19 @@
         <v>79</v>
       </c>
       <c r="B74" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="C74" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D74" t="s">
-        <v>236</v>
+        <v>151</v>
       </c>
       <c r="E74" t="s">
-        <v>259</v>
+        <v>174</v>
       </c>
       <c r="G74" t="s">
-        <v>241</v>
+        <v>156</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -2519,19 +2376,19 @@
         <v>80</v>
       </c>
       <c r="B75" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="C75" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D75" t="s">
-        <v>236</v>
+        <v>151</v>
       </c>
       <c r="E75" t="s">
-        <v>259</v>
+        <v>174</v>
       </c>
       <c r="G75" t="s">
-        <v>241</v>
+        <v>156</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -2539,19 +2396,19 @@
         <v>81</v>
       </c>
       <c r="B76" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="C76" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D76" t="s">
-        <v>236</v>
+        <v>151</v>
       </c>
       <c r="E76" t="s">
-        <v>259</v>
+        <v>174</v>
       </c>
       <c r="G76" t="s">
-        <v>241</v>
+        <v>156</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -2559,19 +2416,19 @@
         <v>82</v>
       </c>
       <c r="B77" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="C77" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D77" t="s">
-        <v>236</v>
+        <v>151</v>
       </c>
       <c r="E77" t="s">
-        <v>259</v>
+        <v>174</v>
       </c>
       <c r="G77" t="s">
-        <v>241</v>
+        <v>156</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -2579,16 +2436,16 @@
         <v>83</v>
       </c>
       <c r="B78" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="C78" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D78" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E78" t="s">
-        <v>253</v>
+        <v>168</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -2596,16 +2453,16 @@
         <v>84</v>
       </c>
       <c r="B79" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="C79" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D79" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E79" t="s">
-        <v>253</v>
+        <v>168</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -2613,16 +2470,16 @@
         <v>85</v>
       </c>
       <c r="B80" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="C80" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D80" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E80" t="s">
-        <v>253</v>
+        <v>168</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -2630,16 +2487,16 @@
         <v>86</v>
       </c>
       <c r="B81" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="C81" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D81" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E81" t="s">
-        <v>253</v>
+        <v>168</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -2647,16 +2504,16 @@
         <v>87</v>
       </c>
       <c r="B82" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="C82" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D82" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E82" t="s">
-        <v>253</v>
+        <v>168</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -2664,16 +2521,16 @@
         <v>88</v>
       </c>
       <c r="B83" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="C83" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D83" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E83" t="s">
-        <v>253</v>
+        <v>168</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -2681,16 +2538,16 @@
         <v>89</v>
       </c>
       <c r="B84" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="C84" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D84" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E84" t="s">
-        <v>253</v>
+        <v>168</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -2698,16 +2555,16 @@
         <v>90</v>
       </c>
       <c r="B85" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="C85" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D85" t="s">
-        <v>237</v>
+        <v>152</v>
       </c>
       <c r="E85" t="s">
-        <v>253</v>
+        <v>168</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -2715,19 +2572,19 @@
         <v>91</v>
       </c>
       <c r="B86" t="s">
-        <v>228</v>
+        <v>146</v>
       </c>
       <c r="C86" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D86" t="s">
-        <v>233</v>
+        <v>148</v>
       </c>
       <c r="E86" t="s">
         <v>91</v>
       </c>
       <c r="G86" t="s">
-        <v>242</v>
+        <v>157</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -2735,19 +2592,19 @@
         <v>92</v>
       </c>
       <c r="B87" t="s">
-        <v>229</v>
+        <v>201</v>
       </c>
       <c r="C87" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D87" t="s">
-        <v>236</v>
+        <v>151</v>
       </c>
       <c r="E87" t="s">
-        <v>260</v>
+        <v>175</v>
       </c>
       <c r="G87" t="s">
-        <v>242</v>
+        <v>157</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -2755,19 +2612,19 @@
         <v>93</v>
       </c>
       <c r="B88" t="s">
-        <v>230</v>
+        <v>202</v>
       </c>
       <c r="C88" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D88" t="s">
-        <v>236</v>
+        <v>151</v>
       </c>
       <c r="E88" t="s">
-        <v>260</v>
+        <v>175</v>
       </c>
       <c r="G88" t="s">
-        <v>242</v>
+        <v>157</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -2775,19 +2632,19 @@
         <v>94</v>
       </c>
       <c r="B89" t="s">
-        <v>231</v>
+        <v>203</v>
       </c>
       <c r="C89" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D89" t="s">
-        <v>236</v>
+        <v>151</v>
       </c>
       <c r="E89" t="s">
-        <v>260</v>
+        <v>175</v>
       </c>
       <c r="G89" t="s">
-        <v>242</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I have updated topbreaks to SRG but without Summary table topbreaks.
</commit_message>
<xml_diff>
--- a/Forsta_meta.xlsx
+++ b/Forsta_meta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Internal\Tabulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6454B1D-B9C1-4085-8C3B-99A966D7DA8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BF1396-7C69-4327-8ABC-6E4F8CEA5FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1034,7 +1034,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>